<commit_message>
refactor: add longueur max dans les differentes tables
</commit_message>
<xml_diff>
--- a/dictionnaireDonnees.xlsx
+++ b/dictionnaireDonnees.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="vehicule"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="31">
   <si>
     <t>nom</t>
   </si>
@@ -61,16 +61,13 @@
     <t>alphabétique</t>
   </si>
   <si>
-    <t/>
+    <t>string</t>
   </si>
   <si>
     <t>montantLocation</t>
   </si>
   <si>
     <t>montantReparation</t>
-  </si>
-  <si>
-    <t>string</t>
   </si>
   <si>
     <t>adresse</t>
@@ -177,7 +174,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -496,7 +493,7 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -530,7 +527,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
@@ -539,7 +536,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -555,14 +552,14 @@
         <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -571,17 +568,17 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C5" s="6">
         <v>10</v>
@@ -594,10 +591,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="6">
         <v>10</v>
@@ -610,23 +607,23 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="6">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
@@ -635,14 +632,14 @@
         <v>256</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>13</v>
@@ -651,7 +648,7 @@
         <v>256</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -711,14 +708,14 @@
         <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>13</v>
@@ -727,14 +724,14 @@
         <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -743,14 +740,14 @@
         <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
@@ -759,14 +756,14 @@
         <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
@@ -775,7 +772,7 @@
         <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -835,14 +832,14 @@
         <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>13</v>
@@ -851,7 +848,7 @@
         <v>100</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -868,7 +865,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -907,7 +904,9 @@
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="3">
+        <v>6</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
@@ -921,7 +920,9 @@
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="3">
+        <v>14</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
@@ -936,7 +937,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="2"/>
@@ -949,7 +950,9 @@
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="3">
+        <v>6</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
@@ -963,7 +966,9 @@
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="3">
+        <v>6</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>